<commit_message>
Perf improvement, additional detailed figures
</commit_message>
<xml_diff>
--- a/plotting_scripts/szeged_data/coronamonitornewcases.xlsx
+++ b/plotting_scripts/szeged_data/coronamonitornewcases.xlsx
@@ -5982,804 +5982,2058 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="3"/>
-      <c r="B409" s="3"/>
-      <c r="C409" s="3"/>
+      <c r="A409" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44301.0)</f>
+        <v>44301</v>
+      </c>
+      <c r="B409" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5307.0)</f>
+        <v>5307</v>
+      </c>
+      <c r="C409" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5498.857142857143)</f>
+        <v>5498.857143</v>
+      </c>
     </row>
     <row r="410">
-      <c r="A410" s="3"/>
-      <c r="B410" s="3"/>
-      <c r="C410" s="3"/>
+      <c r="A410" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44302.0)</f>
+        <v>44302</v>
+      </c>
+      <c r="B410" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5216.0)</f>
+        <v>5216</v>
+      </c>
+      <c r="C410" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5197.571428571428)</f>
+        <v>5197.571429</v>
+      </c>
     </row>
     <row r="411">
-      <c r="A411" s="3"/>
-      <c r="B411" s="3"/>
-      <c r="C411" s="3"/>
+      <c r="A411" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44303.0)</f>
+        <v>44303</v>
+      </c>
+      <c r="B411" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4604.0)</f>
+        <v>4604</v>
+      </c>
+      <c r="C411" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4704.857142857143)</f>
+        <v>4704.857143</v>
+      </c>
     </row>
     <row r="412">
-      <c r="A412" s="3"/>
-      <c r="B412" s="3"/>
-      <c r="C412" s="3"/>
+      <c r="A412" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44304.0)</f>
+        <v>44304</v>
+      </c>
+      <c r="B412" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3706.0)</f>
+        <v>3706</v>
+      </c>
+      <c r="C412" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4334.857142857143)</f>
+        <v>4334.857143</v>
+      </c>
     </row>
     <row r="413">
-      <c r="A413" s="3"/>
-      <c r="B413" s="3"/>
-      <c r="C413" s="3"/>
+      <c r="A413" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44305.0)</f>
+        <v>44305</v>
+      </c>
+      <c r="B413" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2680.0)</f>
+        <v>2680</v>
+      </c>
+      <c r="C413" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3992.4285714285716)</f>
+        <v>3992.428571</v>
+      </c>
     </row>
     <row r="414">
-      <c r="A414" s="3"/>
-      <c r="B414" s="3"/>
-      <c r="C414" s="3"/>
+      <c r="A414" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44306.0)</f>
+        <v>44306</v>
+      </c>
+      <c r="B414" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1645.0)</f>
+        <v>1645</v>
+      </c>
+      <c r="C414" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3822.1428571428573)</f>
+        <v>3822.142857</v>
+      </c>
     </row>
     <row r="415">
-      <c r="A415" s="3"/>
-      <c r="B415" s="3"/>
-      <c r="C415" s="3"/>
+      <c r="A415" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44307.0)</f>
+        <v>44307</v>
+      </c>
+      <c r="B415" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2527.0)</f>
+        <v>2527</v>
+      </c>
+      <c r="C415" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3669.285714285714)</f>
+        <v>3669.285714</v>
+      </c>
     </row>
     <row r="416">
-      <c r="A416" s="3"/>
-      <c r="B416" s="3"/>
-      <c r="C416" s="3"/>
+      <c r="A416" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44308.0)</f>
+        <v>44308</v>
+      </c>
+      <c r="B416" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3607.0)</f>
+        <v>3607</v>
+      </c>
+      <c r="C416" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3426.4285714285716)</f>
+        <v>3426.428571</v>
+      </c>
     </row>
     <row r="417">
-      <c r="A417" s="3"/>
-      <c r="B417" s="3"/>
-      <c r="C417" s="3"/>
+      <c r="A417" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44309.0)</f>
+        <v>44309</v>
+      </c>
+      <c r="B417" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3427.0)</f>
+        <v>3427</v>
+      </c>
+      <c r="C417" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3170.8571428571427)</f>
+        <v>3170.857143</v>
+      </c>
     </row>
     <row r="418">
-      <c r="A418" s="3"/>
-      <c r="B418" s="3"/>
-      <c r="C418" s="3"/>
+      <c r="A418" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44310.0)</f>
+        <v>44310</v>
+      </c>
+      <c r="B418" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2796.0)</f>
+        <v>2796</v>
+      </c>
+      <c r="C418" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2912.5714285714284)</f>
+        <v>2912.571429</v>
+      </c>
     </row>
     <row r="419">
-      <c r="A419" s="3"/>
-      <c r="B419" s="3"/>
-      <c r="C419" s="3"/>
+      <c r="A419" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44311.0)</f>
+        <v>44311</v>
+      </c>
+      <c r="B419" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2328.0)</f>
+        <v>2328</v>
+      </c>
+      <c r="C419" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2715.714285714286)</f>
+        <v>2715.714286</v>
+      </c>
     </row>
     <row r="420">
-      <c r="A420" s="3"/>
-      <c r="B420" s="3"/>
-      <c r="C420" s="3"/>
+      <c r="A420" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44312.0)</f>
+        <v>44312</v>
+      </c>
+      <c r="B420" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1936.0)</f>
+        <v>1936</v>
+      </c>
+      <c r="C420" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2609.4285714285716)</f>
+        <v>2609.428571</v>
+      </c>
     </row>
     <row r="421">
-      <c r="A421" s="3"/>
-      <c r="B421" s="3"/>
-      <c r="C421" s="3"/>
+      <c r="A421" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44313.0)</f>
+        <v>44313</v>
+      </c>
+      <c r="B421" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1253.0)</f>
+        <v>1253</v>
+      </c>
+      <c r="C421" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2553.4285714285716)</f>
+        <v>2553.428571</v>
+      </c>
     </row>
     <row r="422">
-      <c r="A422" s="3"/>
-      <c r="B422" s="3"/>
-      <c r="C422" s="3"/>
+      <c r="A422" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44314.0)</f>
+        <v>44314</v>
+      </c>
+      <c r="B422" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1692.0)</f>
+        <v>1692</v>
+      </c>
+      <c r="C422" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2434.1428571428573)</f>
+        <v>2434.142857</v>
+      </c>
     </row>
     <row r="423">
-      <c r="A423" s="3"/>
-      <c r="B423" s="3"/>
-      <c r="C423" s="3"/>
+      <c r="A423" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44315.0)</f>
+        <v>44315</v>
+      </c>
+      <c r="B423" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2584.0)</f>
+        <v>2584</v>
+      </c>
+      <c r="C423" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2288.0)</f>
+        <v>2288</v>
+      </c>
     </row>
     <row r="424">
-      <c r="A424" s="3"/>
-      <c r="B424" s="3"/>
-      <c r="C424" s="3"/>
+      <c r="A424" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44316.0)</f>
+        <v>44316</v>
+      </c>
+      <c r="B424" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2365.0)</f>
+        <v>2365</v>
+      </c>
+      <c r="C424" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2136.285714285714)</f>
+        <v>2136.285714</v>
+      </c>
     </row>
     <row r="425">
-      <c r="A425" s="3"/>
-      <c r="B425" s="3"/>
-      <c r="C425" s="3"/>
+      <c r="A425" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44317.0)</f>
+        <v>44317</v>
+      </c>
+      <c r="B425" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1951.0)</f>
+        <v>1951</v>
+      </c>
+      <c r="C425" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2015.5714285714287)</f>
+        <v>2015.571429</v>
+      </c>
     </row>
     <row r="426">
-      <c r="A426" s="3"/>
-      <c r="B426" s="3"/>
-      <c r="C426" s="3"/>
+      <c r="A426" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44318.0)</f>
+        <v>44318</v>
+      </c>
+      <c r="B426" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1593.0)</f>
+        <v>1593</v>
+      </c>
+      <c r="C426" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1910.5714285714287)</f>
+        <v>1910.571429</v>
+      </c>
     </row>
     <row r="427">
-      <c r="A427" s="3"/>
-      <c r="B427" s="3"/>
-      <c r="C427" s="3"/>
+      <c r="A427" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44319.0)</f>
+        <v>44319</v>
+      </c>
+      <c r="B427" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1219.0)</f>
+        <v>1219</v>
+      </c>
+      <c r="C427" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1808.142857142857)</f>
+        <v>1808.142857</v>
+      </c>
     </row>
     <row r="428">
-      <c r="A428" s="3"/>
-      <c r="B428" s="3"/>
-      <c r="C428" s="3"/>
+      <c r="A428" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44320.0)</f>
+        <v>44320</v>
+      </c>
+      <c r="B428" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),726.0)</f>
+        <v>726</v>
+      </c>
+      <c r="C428" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1732.857142857143)</f>
+        <v>1732.857143</v>
+      </c>
     </row>
     <row r="429">
-      <c r="A429" s="3"/>
-      <c r="B429" s="3"/>
-      <c r="C429" s="3"/>
+      <c r="A429" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44321.0)</f>
+        <v>44321</v>
+      </c>
+      <c r="B429" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1130.0)</f>
+        <v>1130</v>
+      </c>
+      <c r="C429" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1652.5714285714287)</f>
+        <v>1652.571429</v>
+      </c>
     </row>
     <row r="430">
-      <c r="A430" s="3"/>
-      <c r="B430" s="3"/>
-      <c r="C430" s="3"/>
+      <c r="A430" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44322.0)</f>
+        <v>44322</v>
+      </c>
+      <c r="B430" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1680.0)</f>
+        <v>1680</v>
+      </c>
+      <c r="C430" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1523.4285714285713)</f>
+        <v>1523.428571</v>
+      </c>
     </row>
     <row r="431">
-      <c r="A431" s="3"/>
-      <c r="B431" s="3"/>
-      <c r="C431" s="3"/>
+      <c r="A431" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44323.0)</f>
+        <v>44323</v>
+      </c>
+      <c r="B431" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1541.0)</f>
+        <v>1541</v>
+      </c>
+      <c r="C431" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1405.7142857142858)</f>
+        <v>1405.714286</v>
+      </c>
     </row>
     <row r="432">
-      <c r="A432" s="3"/>
-      <c r="B432" s="3"/>
-      <c r="C432" s="3"/>
+      <c r="A432" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44324.0)</f>
+        <v>44324</v>
+      </c>
+      <c r="B432" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1376.0)</f>
+        <v>1376</v>
+      </c>
+      <c r="C432" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1323.5714285714287)</f>
+        <v>1323.571429</v>
+      </c>
     </row>
     <row r="433">
-      <c r="A433" s="3"/>
-      <c r="B433" s="3"/>
-      <c r="C433" s="3"/>
+      <c r="A433" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44325.0)</f>
+        <v>44325</v>
+      </c>
+      <c r="B433" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1145.0)</f>
+        <v>1145</v>
+      </c>
+      <c r="C433" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1259.5714285714287)</f>
+        <v>1259.571429</v>
+      </c>
     </row>
     <row r="434">
-      <c r="A434" s="3"/>
-      <c r="B434" s="3"/>
-      <c r="C434" s="3"/>
+      <c r="A434" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44326.0)</f>
+        <v>44326</v>
+      </c>
+      <c r="B434" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),677.0)</f>
+        <v>677</v>
+      </c>
+      <c r="C434" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1182.142857142857)</f>
+        <v>1182.142857</v>
+      </c>
     </row>
     <row r="435">
-      <c r="A435" s="3"/>
-      <c r="B435" s="3"/>
-      <c r="C435" s="3"/>
+      <c r="A435" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44327.0)</f>
+        <v>44327</v>
+      </c>
+      <c r="B435" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),493.0)</f>
+        <v>493</v>
+      </c>
+      <c r="C435" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1148.857142857143)</f>
+        <v>1148.857143</v>
+      </c>
     </row>
     <row r="436">
-      <c r="A436" s="3"/>
-      <c r="B436" s="3"/>
-      <c r="C436" s="3"/>
+      <c r="A436" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44328.0)</f>
+        <v>44328</v>
+      </c>
+      <c r="B436" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),905.0)</f>
+        <v>905</v>
+      </c>
+      <c r="C436" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1116.7142857142858)</f>
+        <v>1116.714286</v>
+      </c>
     </row>
     <row r="437">
-      <c r="A437" s="3"/>
-      <c r="B437" s="3"/>
-      <c r="C437" s="3"/>
+      <c r="A437" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44329.0)</f>
+        <v>44329</v>
+      </c>
+      <c r="B437" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1416.0)</f>
+        <v>1416</v>
+      </c>
+      <c r="C437" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1079.0)</f>
+        <v>1079</v>
+      </c>
     </row>
     <row r="438">
-      <c r="A438" s="3"/>
-      <c r="B438" s="3"/>
-      <c r="C438" s="3"/>
+      <c r="A438" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44330.0)</f>
+        <v>44330</v>
+      </c>
+      <c r="B438" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1190.0)</f>
+        <v>1190</v>
+      </c>
+      <c r="C438" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1028.857142857143)</f>
+        <v>1028.857143</v>
+      </c>
     </row>
     <row r="439">
-      <c r="A439" s="3"/>
-      <c r="B439" s="3"/>
-      <c r="C439" s="3"/>
+      <c r="A439" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44331.0)</f>
+        <v>44331</v>
+      </c>
+      <c r="B439" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1039.0)</f>
+        <v>1039</v>
+      </c>
+      <c r="C439" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),980.7142857142857)</f>
+        <v>980.7142857</v>
+      </c>
     </row>
     <row r="440">
-      <c r="A440" s="3"/>
-      <c r="B440" s="3"/>
-      <c r="C440" s="3"/>
+      <c r="A440" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44332.0)</f>
+        <v>44332</v>
+      </c>
+      <c r="B440" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),718.0)</f>
+        <v>718</v>
+      </c>
+      <c r="C440" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),919.7142857142857)</f>
+        <v>919.7142857</v>
+      </c>
     </row>
     <row r="441">
-      <c r="A441" s="3"/>
-      <c r="B441" s="3"/>
-      <c r="C441" s="3"/>
+      <c r="A441" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44333.0)</f>
+        <v>44333</v>
+      </c>
+      <c r="B441" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),426.0)</f>
+        <v>426</v>
+      </c>
+      <c r="C441" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),883.8571428571429)</f>
+        <v>883.8571429</v>
+      </c>
     </row>
     <row r="442">
-      <c r="A442" s="3"/>
-      <c r="B442" s="3"/>
-      <c r="C442" s="3"/>
+      <c r="A442" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44334.0)</f>
+        <v>44334</v>
+      </c>
+      <c r="B442" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),382.0)</f>
+        <v>382</v>
+      </c>
+      <c r="C442" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),868.0)</f>
+        <v>868</v>
+      </c>
     </row>
     <row r="443">
-      <c r="A443" s="3"/>
-      <c r="B443" s="3"/>
-      <c r="C443" s="3"/>
+      <c r="A443" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44335.0)</f>
+        <v>44335</v>
+      </c>
+      <c r="B443" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),633.0)</f>
+        <v>633</v>
+      </c>
+      <c r="C443" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),829.1428571428571)</f>
+        <v>829.1428571</v>
+      </c>
     </row>
     <row r="444">
-      <c r="A444" s="3"/>
-      <c r="B444" s="3"/>
-      <c r="C444" s="3"/>
+      <c r="A444" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44336.0)</f>
+        <v>44336</v>
+      </c>
+      <c r="B444" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),780.0)</f>
+        <v>780</v>
+      </c>
+      <c r="C444" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),738.2857142857143)</f>
+        <v>738.2857143</v>
+      </c>
     </row>
     <row r="445">
-      <c r="A445" s="3"/>
-      <c r="B445" s="3"/>
-      <c r="C445" s="3"/>
+      <c r="A445" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44337.0)</f>
+        <v>44337</v>
+      </c>
+      <c r="B445" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),657.0)</f>
+        <v>657</v>
+      </c>
+      <c r="C445" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),662.1428571428571)</f>
+        <v>662.1428571</v>
+      </c>
     </row>
     <row r="446">
-      <c r="A446" s="3"/>
-      <c r="B446" s="3"/>
-      <c r="C446" s="3"/>
+      <c r="A446" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44338.0)</f>
+        <v>44338</v>
+      </c>
+      <c r="B446" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),647.0)</f>
+        <v>647</v>
+      </c>
+      <c r="C446" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),606.1428571428571)</f>
+        <v>606.1428571</v>
+      </c>
     </row>
     <row r="447">
-      <c r="A447" s="3"/>
-      <c r="B447" s="3"/>
-      <c r="C447" s="3"/>
+      <c r="A447" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44339.0)</f>
+        <v>44339</v>
+      </c>
+      <c r="B447" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),416.0)</f>
+        <v>416</v>
+      </c>
+      <c r="C447" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),563.0)</f>
+        <v>563</v>
+      </c>
     </row>
     <row r="448">
-      <c r="A448" s="3"/>
-      <c r="B448" s="3"/>
-      <c r="C448" s="3"/>
+      <c r="A448" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44340.0)</f>
+        <v>44340</v>
+      </c>
+      <c r="B448" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),258.0)</f>
+        <v>258</v>
+      </c>
+      <c r="C448" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),539.0)</f>
+        <v>539</v>
+      </c>
     </row>
     <row r="449">
-      <c r="A449" s="3"/>
-      <c r="B449" s="3"/>
-      <c r="C449" s="3"/>
+      <c r="A449" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44341.0)</f>
+        <v>44341</v>
+      </c>
+      <c r="B449" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),164.0)</f>
+        <v>164</v>
+      </c>
+      <c r="C449" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),507.85714285714283)</f>
+        <v>507.8571429</v>
+      </c>
     </row>
     <row r="450">
-      <c r="A450" s="3"/>
-      <c r="B450" s="3"/>
-      <c r="C450" s="3"/>
+      <c r="A450" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44342.0)</f>
+        <v>44342</v>
+      </c>
+      <c r="B450" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),213.0)</f>
+        <v>213</v>
+      </c>
+      <c r="C450" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),447.85714285714283)</f>
+        <v>447.8571429</v>
+      </c>
     </row>
     <row r="451">
-      <c r="A451" s="3"/>
-      <c r="B451" s="3"/>
-      <c r="C451" s="3"/>
+      <c r="A451" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44343.0)</f>
+        <v>44343</v>
+      </c>
+      <c r="B451" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),396.0)</f>
+        <v>396</v>
+      </c>
+      <c r="C451" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),393.0)</f>
+        <v>393</v>
+      </c>
     </row>
     <row r="452">
-      <c r="A452" s="3"/>
-      <c r="B452" s="3"/>
-      <c r="C452" s="3"/>
+      <c r="A452" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44344.0)</f>
+        <v>44344</v>
+      </c>
+      <c r="B452" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),448.0)</f>
+        <v>448</v>
+      </c>
+      <c r="C452" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),363.14285714285717)</f>
+        <v>363.1428571</v>
+      </c>
     </row>
     <row r="453">
-      <c r="A453" s="3"/>
-      <c r="B453" s="3"/>
-      <c r="C453" s="3"/>
+      <c r="A453" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44345.0)</f>
+        <v>44345</v>
+      </c>
+      <c r="B453" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),465.0)</f>
+        <v>465</v>
+      </c>
+      <c r="C453" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),337.14285714285717)</f>
+        <v>337.1428571</v>
+      </c>
     </row>
     <row r="454">
-      <c r="A454" s="3"/>
-      <c r="B454" s="3"/>
-      <c r="C454" s="3"/>
+      <c r="A454" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44346.0)</f>
+        <v>44346</v>
+      </c>
+      <c r="B454" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),350.0)</f>
+        <v>350</v>
+      </c>
+      <c r="C454" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),327.7142857142857)</f>
+        <v>327.7142857</v>
+      </c>
     </row>
     <row r="455">
-      <c r="A455" s="3"/>
-      <c r="B455" s="3"/>
-      <c r="C455" s="3"/>
+      <c r="A455" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44347.0)</f>
+        <v>44347</v>
+      </c>
+      <c r="B455" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),156.0)</f>
+        <v>156</v>
+      </c>
+      <c r="C455" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),313.14285714285717)</f>
+        <v>313.1428571</v>
+      </c>
     </row>
     <row r="456">
-      <c r="A456" s="3"/>
-      <c r="B456" s="3"/>
-      <c r="C456" s="3"/>
+      <c r="A456" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44348.0)</f>
+        <v>44348</v>
+      </c>
+      <c r="B456" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),174.0)</f>
+        <v>174</v>
+      </c>
+      <c r="C456" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),314.57142857142856)</f>
+        <v>314.5714286</v>
+      </c>
     </row>
     <row r="457">
-      <c r="A457" s="3"/>
-      <c r="B457" s="3"/>
-      <c r="C457" s="3"/>
+      <c r="A457" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44349.0)</f>
+        <v>44349</v>
+      </c>
+      <c r="B457" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),275.0)</f>
+        <v>275</v>
+      </c>
+      <c r="C457" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),323.42857142857144)</f>
+        <v>323.4285714</v>
+      </c>
     </row>
     <row r="458">
-      <c r="A458" s="3"/>
-      <c r="B458" s="3"/>
-      <c r="C458" s="3"/>
+      <c r="A458" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44350.0)</f>
+        <v>44350</v>
+      </c>
+      <c r="B458" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),315.0)</f>
+        <v>315</v>
+      </c>
+      <c r="C458" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),311.85714285714283)</f>
+        <v>311.8571429</v>
+      </c>
     </row>
     <row r="459">
-      <c r="A459" s="3"/>
-      <c r="B459" s="3"/>
-      <c r="C459" s="3"/>
+      <c r="A459" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44351.0)</f>
+        <v>44351</v>
+      </c>
+      <c r="B459" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),269.0)</f>
+        <v>269</v>
+      </c>
+      <c r="C459" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),286.2857142857143)</f>
+        <v>286.2857143</v>
+      </c>
     </row>
     <row r="460">
-      <c r="A460" s="3"/>
-      <c r="B460" s="3"/>
-      <c r="C460" s="3"/>
+      <c r="A460" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44352.0)</f>
+        <v>44352</v>
+      </c>
+      <c r="B460" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),300.0)</f>
+        <v>300</v>
+      </c>
+      <c r="C460" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),262.7142857142857)</f>
+        <v>262.7142857</v>
+      </c>
     </row>
     <row r="461">
-      <c r="A461" s="3"/>
-      <c r="B461" s="3"/>
-      <c r="C461" s="3"/>
+      <c r="A461" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44353.0)</f>
+        <v>44353</v>
+      </c>
+      <c r="B461" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),137.0)</f>
+        <v>137</v>
+      </c>
+      <c r="C461" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),232.28571428571428)</f>
+        <v>232.2857143</v>
+      </c>
     </row>
     <row r="462">
-      <c r="A462" s="3"/>
-      <c r="B462" s="3"/>
-      <c r="C462" s="3"/>
+      <c r="A462" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44354.0)</f>
+        <v>44354</v>
+      </c>
+      <c r="B462" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),81.0)</f>
+        <v>81</v>
+      </c>
+      <c r="C462" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),221.57142857142858)</f>
+        <v>221.5714286</v>
+      </c>
     </row>
     <row r="463">
-      <c r="A463" s="3"/>
-      <c r="B463" s="3"/>
-      <c r="C463" s="3"/>
+      <c r="A463" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44355.0)</f>
+        <v>44355</v>
+      </c>
+      <c r="B463" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),117.0)</f>
+        <v>117</v>
+      </c>
+      <c r="C463" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),213.42857142857142)</f>
+        <v>213.4285714</v>
+      </c>
     </row>
     <row r="464">
-      <c r="A464" s="3"/>
-      <c r="B464" s="3"/>
-      <c r="C464" s="3"/>
+      <c r="A464" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44356.0)</f>
+        <v>44356</v>
+      </c>
+      <c r="B464" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),179.0)</f>
+        <v>179</v>
+      </c>
+      <c r="C464" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),199.71428571428572)</f>
+        <v>199.7142857</v>
+      </c>
     </row>
     <row r="465">
-      <c r="A465" s="3"/>
-      <c r="B465" s="3"/>
-      <c r="C465" s="3"/>
+      <c r="A465" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44357.0)</f>
+        <v>44357</v>
+      </c>
+      <c r="B465" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),206.0)</f>
+        <v>206</v>
+      </c>
+      <c r="C465" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),184.14285714285714)</f>
+        <v>184.1428571</v>
+      </c>
     </row>
     <row r="466">
-      <c r="A466" s="3"/>
-      <c r="B466" s="3"/>
-      <c r="C466" s="3"/>
+      <c r="A466" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44358.0)</f>
+        <v>44358</v>
+      </c>
+      <c r="B466" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),199.0)</f>
+        <v>199</v>
+      </c>
+      <c r="C466" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),174.14285714285714)</f>
+        <v>174.1428571</v>
+      </c>
     </row>
     <row r="467">
-      <c r="A467" s="3"/>
+      <c r="A467" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44359.0)</f>
+        <v>44359</v>
+      </c>
       <c r="B467" s="3"/>
       <c r="C467" s="3"/>
     </row>
     <row r="468">
-      <c r="A468" s="3"/>
+      <c r="A468" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44360.0)</f>
+        <v>44360</v>
+      </c>
       <c r="B468" s="3"/>
       <c r="C468" s="3"/>
     </row>
     <row r="469">
-      <c r="A469" s="3"/>
-      <c r="B469" s="3"/>
-      <c r="C469" s="3"/>
+      <c r="A469" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44361.0)</f>
+        <v>44361</v>
+      </c>
+      <c r="B469" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),255.0)</f>
+        <v>255</v>
+      </c>
+      <c r="C469" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),136.57142857142858)</f>
+        <v>136.5714286</v>
+      </c>
     </row>
     <row r="470">
-      <c r="A470" s="3"/>
-      <c r="B470" s="3"/>
-      <c r="C470" s="3"/>
+      <c r="A470" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44362.0)</f>
+        <v>44362</v>
+      </c>
+      <c r="B470" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),57.0)</f>
+        <v>57</v>
+      </c>
+      <c r="C470" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),128.0)</f>
+        <v>128</v>
+      </c>
     </row>
     <row r="471">
-      <c r="A471" s="3"/>
-      <c r="B471" s="3"/>
-      <c r="C471" s="3"/>
+      <c r="A471" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44363.0)</f>
+        <v>44363</v>
+      </c>
+      <c r="B471" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),107.0)</f>
+        <v>107</v>
+      </c>
+      <c r="C471" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),117.71428571428571)</f>
+        <v>117.7142857</v>
+      </c>
     </row>
     <row r="472">
-      <c r="A472" s="3"/>
-      <c r="B472" s="3"/>
-      <c r="C472" s="3"/>
+      <c r="A472" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44364.0)</f>
+        <v>44364</v>
+      </c>
+      <c r="B472" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),113.0)</f>
+        <v>113</v>
+      </c>
+      <c r="C472" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),104.42857142857143)</f>
+        <v>104.4285714</v>
+      </c>
     </row>
     <row r="473">
-      <c r="A473" s="3"/>
-      <c r="B473" s="3"/>
-      <c r="C473" s="3"/>
+      <c r="A473" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44365.0)</f>
+        <v>44365</v>
+      </c>
+      <c r="B473" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),106.0)</f>
+        <v>106</v>
+      </c>
+      <c r="C473" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),91.14285714285714)</f>
+        <v>91.14285714</v>
+      </c>
     </row>
     <row r="474">
-      <c r="A474" s="3"/>
+      <c r="A474" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44366.0)</f>
+        <v>44366</v>
+      </c>
       <c r="B474" s="3"/>
       <c r="C474" s="3"/>
     </row>
     <row r="475">
-      <c r="A475" s="3"/>
+      <c r="A475" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44367.0)</f>
+        <v>44367</v>
+      </c>
       <c r="B475" s="3"/>
       <c r="C475" s="3"/>
     </row>
     <row r="476">
-      <c r="A476" s="3"/>
-      <c r="B476" s="3"/>
-      <c r="C476" s="3"/>
+      <c r="A476" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44368.0)</f>
+        <v>44368</v>
+      </c>
+      <c r="B476" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),202.0)</f>
+        <v>202</v>
+      </c>
+      <c r="C476" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.57142857142857)</f>
+        <v>83.57142857</v>
+      </c>
     </row>
     <row r="477">
-      <c r="A477" s="3"/>
-      <c r="B477" s="3"/>
-      <c r="C477" s="3"/>
+      <c r="A477" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44369.0)</f>
+        <v>44369</v>
+      </c>
+      <c r="B477" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.0)</f>
+        <v>54</v>
+      </c>
+      <c r="C477" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.14285714285714)</f>
+        <v>83.14285714</v>
+      </c>
     </row>
     <row r="478">
-      <c r="A478" s="3"/>
-      <c r="B478" s="3"/>
-      <c r="C478" s="3"/>
+      <c r="A478" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44370.0)</f>
+        <v>44370</v>
+      </c>
+      <c r="B478" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),91.0)</f>
+        <v>91</v>
+      </c>
+      <c r="C478" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),80.85714285714286)</f>
+        <v>80.85714286</v>
+      </c>
     </row>
     <row r="479">
-      <c r="A479" s="3"/>
-      <c r="B479" s="3"/>
-      <c r="C479" s="3"/>
+      <c r="A479" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44371.0)</f>
+        <v>44371</v>
+      </c>
+      <c r="B479" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69.0)</f>
+        <v>69</v>
+      </c>
+      <c r="C479" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.57142857142857)</f>
+        <v>74.57142857</v>
+      </c>
     </row>
     <row r="480">
-      <c r="A480" s="3"/>
-      <c r="B480" s="3"/>
-      <c r="C480" s="3"/>
+      <c r="A480" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44372.0)</f>
+        <v>44372</v>
+      </c>
+      <c r="B480" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),66.0)</f>
+        <v>66</v>
+      </c>
+      <c r="C480" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),68.85714285714286)</f>
+        <v>68.85714286</v>
+      </c>
     </row>
     <row r="481">
-      <c r="A481" s="3"/>
+      <c r="A481" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44373.0)</f>
+        <v>44373</v>
+      </c>
       <c r="B481" s="3"/>
       <c r="C481" s="3"/>
     </row>
     <row r="482">
-      <c r="A482" s="3"/>
+      <c r="A482" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44374.0)</f>
+        <v>44374</v>
+      </c>
       <c r="B482" s="3"/>
       <c r="C482" s="3"/>
     </row>
     <row r="483">
-      <c r="A483" s="3"/>
-      <c r="B483" s="3"/>
-      <c r="C483" s="3"/>
+      <c r="A483" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44375.0)</f>
+        <v>44375</v>
+      </c>
+      <c r="B483" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),132.0)</f>
+        <v>132</v>
+      </c>
+      <c r="C483" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58.857142857142854)</f>
+        <v>58.85714286</v>
+      </c>
     </row>
     <row r="484">
-      <c r="A484" s="3"/>
-      <c r="B484" s="3"/>
-      <c r="C484" s="3"/>
+      <c r="A484" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44376.0)</f>
+        <v>44376</v>
+      </c>
+      <c r="B484" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
+        <v>34</v>
+      </c>
+      <c r="C484" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.0)</f>
+        <v>56</v>
+      </c>
     </row>
     <row r="485">
-      <c r="A485" s="3"/>
-      <c r="B485" s="3"/>
-      <c r="C485" s="3"/>
+      <c r="A485" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44377.0)</f>
+        <v>44377</v>
+      </c>
+      <c r="B485" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.0)</f>
+        <v>52</v>
+      </c>
+      <c r="C485" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.42857142857143)</f>
+        <v>50.42857143</v>
+      </c>
     </row>
     <row r="486">
-      <c r="A486" s="3"/>
-      <c r="B486" s="3"/>
-      <c r="C486" s="3"/>
+      <c r="A486" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44378.0)</f>
+        <v>44378</v>
+      </c>
+      <c r="B486" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
+        <v>32</v>
+      </c>
+      <c r="C486" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45.142857142857146)</f>
+        <v>45.14285714</v>
+      </c>
     </row>
     <row r="487">
-      <c r="A487" s="3"/>
-      <c r="B487" s="3"/>
-      <c r="C487" s="3"/>
+      <c r="A487" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44379.0)</f>
+        <v>44379</v>
+      </c>
+      <c r="B487" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),37.0)</f>
+        <v>37</v>
+      </c>
+      <c r="C487" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.0)</f>
+        <v>41</v>
+      </c>
     </row>
     <row r="488">
-      <c r="A488" s="3"/>
+      <c r="A488" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44380.0)</f>
+        <v>44380</v>
+      </c>
       <c r="B488" s="3"/>
       <c r="C488" s="3"/>
     </row>
     <row r="489">
-      <c r="A489" s="3"/>
+      <c r="A489" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44381.0)</f>
+        <v>44381</v>
+      </c>
       <c r="B489" s="3"/>
       <c r="C489" s="3"/>
     </row>
     <row r="490">
-      <c r="A490" s="3"/>
-      <c r="B490" s="3"/>
-      <c r="C490" s="3"/>
+      <c r="A490" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44382.0)</f>
+        <v>44382</v>
+      </c>
+      <c r="B490" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
+        <v>65</v>
+      </c>
+      <c r="C490" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.428571428571427)</f>
+        <v>31.42857143</v>
+      </c>
     </row>
     <row r="491">
-      <c r="A491" s="3"/>
-      <c r="B491" s="3"/>
-      <c r="C491" s="3"/>
+      <c r="A491" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44383.0)</f>
+        <v>44383</v>
+      </c>
+      <c r="B491" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
+        <v>32</v>
+      </c>
+      <c r="C491" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.142857142857142)</f>
+        <v>31.14285714</v>
+      </c>
     </row>
     <row r="492">
-      <c r="A492" s="3"/>
-      <c r="B492" s="3"/>
-      <c r="C492" s="3"/>
+      <c r="A492" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44384.0)</f>
+        <v>44384</v>
+      </c>
+      <c r="B492" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
+        <v>44</v>
+      </c>
+      <c r="C492" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),30.0)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="493">
-      <c r="A493" s="3"/>
-      <c r="B493" s="3"/>
-      <c r="C493" s="3"/>
+      <c r="A493" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44385.0)</f>
+        <v>44385</v>
+      </c>
+      <c r="B493" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),55.0)</f>
+        <v>55</v>
+      </c>
+      <c r="C493" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.285714285714285)</f>
+        <v>33.28571429</v>
+      </c>
     </row>
     <row r="494">
-      <c r="A494" s="3"/>
-      <c r="B494" s="3"/>
-      <c r="C494" s="3"/>
+      <c r="A494" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44386.0)</f>
+        <v>44386</v>
+      </c>
+      <c r="B494" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
+        <v>44</v>
+      </c>
+      <c r="C494" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.285714285714285)</f>
+        <v>34.28571429</v>
+      </c>
     </row>
     <row r="495">
-      <c r="A495" s="3"/>
+      <c r="A495" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44387.0)</f>
+        <v>44387</v>
+      </c>
       <c r="B495" s="3"/>
       <c r="C495" s="3"/>
     </row>
     <row r="496">
-      <c r="A496" s="3"/>
+      <c r="A496" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44388.0)</f>
+        <v>44388</v>
+      </c>
       <c r="B496" s="3"/>
       <c r="C496" s="3"/>
     </row>
     <row r="497">
-      <c r="A497" s="3"/>
-      <c r="B497" s="3"/>
-      <c r="C497" s="3"/>
+      <c r="A497" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44389.0)</f>
+        <v>44389</v>
+      </c>
+      <c r="B497" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),102.0)</f>
+        <v>102</v>
+      </c>
+      <c r="C497" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),39.57142857142857)</f>
+        <v>39.57142857</v>
+      </c>
     </row>
     <row r="498">
-      <c r="A498" s="3"/>
-      <c r="B498" s="3"/>
-      <c r="C498" s="3"/>
+      <c r="A498" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44390.0)</f>
+        <v>44390</v>
+      </c>
+      <c r="B498" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),17.0)</f>
+        <v>17</v>
+      </c>
+      <c r="C498" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),37.42857142857143)</f>
+        <v>37.42857143</v>
+      </c>
     </row>
     <row r="499">
-      <c r="A499" s="3"/>
-      <c r="B499" s="3"/>
-      <c r="C499" s="3"/>
+      <c r="A499" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44391.0)</f>
+        <v>44391</v>
+      </c>
+      <c r="B499" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.0)</f>
+        <v>56</v>
+      </c>
+      <c r="C499" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),39.142857142857146)</f>
+        <v>39.14285714</v>
+      </c>
     </row>
     <row r="500">
-      <c r="A500" s="3"/>
-      <c r="B500" s="3"/>
-      <c r="C500" s="3"/>
+      <c r="A500" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44392.0)</f>
+        <v>44392</v>
+      </c>
+      <c r="B500" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),49.0)</f>
+        <v>49</v>
+      </c>
+      <c r="C500" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.285714285714285)</f>
+        <v>38.28571429</v>
+      </c>
     </row>
     <row r="501">
-      <c r="A501" s="3"/>
-      <c r="B501" s="3"/>
-      <c r="C501" s="3"/>
+      <c r="A501" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44393.0)</f>
+        <v>44393</v>
+      </c>
+      <c r="B501" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),64.0)</f>
+        <v>64</v>
+      </c>
+      <c r="C501" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.142857142857146)</f>
+        <v>41.14285714</v>
+      </c>
     </row>
     <row r="502">
-      <c r="A502" s="3"/>
+      <c r="A502" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44394.0)</f>
+        <v>44394</v>
+      </c>
       <c r="B502" s="3"/>
       <c r="C502" s="3"/>
     </row>
     <row r="503">
-      <c r="A503" s="3"/>
+      <c r="A503" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44395.0)</f>
+        <v>44395</v>
+      </c>
       <c r="B503" s="3"/>
       <c r="C503" s="3"/>
     </row>
     <row r="504">
-      <c r="A504" s="3"/>
-      <c r="B504" s="3"/>
-      <c r="C504" s="3"/>
+      <c r="A504" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44396.0)</f>
+        <v>44396</v>
+      </c>
+      <c r="B504" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),139.0)</f>
+        <v>139</v>
+      </c>
+      <c r="C504" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.42857142857143)</f>
+        <v>46.42857143</v>
+      </c>
     </row>
     <row r="505">
-      <c r="A505" s="3"/>
-      <c r="B505" s="3"/>
-      <c r="C505" s="3"/>
+      <c r="A505" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44397.0)</f>
+        <v>44397</v>
+      </c>
+      <c r="B505" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
+        <v>25</v>
+      </c>
+      <c r="C505" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),47.57142857142857)</f>
+        <v>47.57142857</v>
+      </c>
     </row>
     <row r="506">
-      <c r="A506" s="3"/>
-      <c r="B506" s="3"/>
-      <c r="C506" s="3"/>
+      <c r="A506" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44398.0)</f>
+        <v>44398</v>
+      </c>
+      <c r="B506" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.0)</f>
+        <v>56</v>
+      </c>
+      <c r="C506" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),47.57142857142857)</f>
+        <v>47.57142857</v>
+      </c>
     </row>
     <row r="507">
-      <c r="A507" s="3"/>
-      <c r="B507" s="3"/>
-      <c r="C507" s="3"/>
+      <c r="A507" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44399.0)</f>
+        <v>44399</v>
+      </c>
+      <c r="B507" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
+        <v>71</v>
+      </c>
+      <c r="C507" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),50.714285714285715)</f>
+        <v>50.71428571</v>
+      </c>
     </row>
     <row r="508">
-      <c r="A508" s="3"/>
-      <c r="B508" s="3"/>
-      <c r="C508" s="3"/>
+      <c r="A508" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44400.0)</f>
+        <v>44400</v>
+      </c>
+      <c r="B508" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),85.0)</f>
+        <v>85</v>
+      </c>
+      <c r="C508" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),53.714285714285715)</f>
+        <v>53.71428571</v>
+      </c>
     </row>
     <row r="509">
-      <c r="A509" s="3"/>
+      <c r="A509" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44401.0)</f>
+        <v>44401</v>
+      </c>
       <c r="B509" s="3"/>
       <c r="C509" s="3"/>
     </row>
     <row r="510">
-      <c r="A510" s="3"/>
+      <c r="A510" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44402.0)</f>
+        <v>44402</v>
+      </c>
       <c r="B510" s="3"/>
       <c r="C510" s="3"/>
     </row>
     <row r="511">
-      <c r="A511" s="3"/>
-      <c r="B511" s="3"/>
-      <c r="C511" s="3"/>
+      <c r="A511" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44403.0)</f>
+        <v>44403</v>
+      </c>
+      <c r="B511" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),161.0)</f>
+        <v>161</v>
+      </c>
+      <c r="C511" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.857142857142854)</f>
+        <v>56.85714286</v>
+      </c>
     </row>
     <row r="512">
-      <c r="A512" s="3"/>
-      <c r="B512" s="3"/>
-      <c r="C512" s="3"/>
+      <c r="A512" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44404.0)</f>
+        <v>44404</v>
+      </c>
+      <c r="B512" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.0)</f>
+        <v>26</v>
+      </c>
+      <c r="C512" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),57.0)</f>
+        <v>57</v>
+      </c>
     </row>
     <row r="513">
-      <c r="A513" s="3"/>
-      <c r="B513" s="3"/>
-      <c r="C513" s="3"/>
+      <c r="A513" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44405.0)</f>
+        <v>44405</v>
+      </c>
+      <c r="B513" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.0)</f>
+        <v>74</v>
+      </c>
+      <c r="C513" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),59.57142857142857)</f>
+        <v>59.57142857</v>
+      </c>
     </row>
     <row r="514">
-      <c r="A514" s="3"/>
-      <c r="B514" s="3"/>
-      <c r="C514" s="3"/>
+      <c r="A514" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44406.0)</f>
+        <v>44406</v>
+      </c>
+      <c r="B514" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
+        <v>65</v>
+      </c>
+      <c r="C514" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58.714285714285715)</f>
+        <v>58.71428571</v>
+      </c>
     </row>
     <row r="515">
-      <c r="A515" s="3"/>
-      <c r="B515" s="3"/>
-      <c r="C515" s="3"/>
+      <c r="A515" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44407.0)</f>
+        <v>44407</v>
+      </c>
+      <c r="B515" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),64.0)</f>
+        <v>64</v>
+      </c>
+      <c r="C515" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),55.714285714285715)</f>
+        <v>55.71428571</v>
+      </c>
     </row>
     <row r="516">
-      <c r="A516" s="3"/>
+      <c r="A516" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44408.0)</f>
+        <v>44408</v>
+      </c>
       <c r="B516" s="3"/>
       <c r="C516" s="3"/>
     </row>
     <row r="517">
-      <c r="A517" s="3"/>
+      <c r="A517" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44409.0)</f>
+        <v>44409</v>
+      </c>
       <c r="B517" s="3"/>
       <c r="C517" s="3"/>
     </row>
     <row r="518">
-      <c r="A518" s="3"/>
-      <c r="B518" s="3"/>
-      <c r="C518" s="3"/>
+      <c r="A518" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44410.0)</f>
+        <v>44410</v>
+      </c>
+      <c r="B518" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),155.0)</f>
+        <v>155</v>
+      </c>
+      <c r="C518" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.857142857142854)</f>
+        <v>54.85714286</v>
+      </c>
     </row>
     <row r="519">
-      <c r="A519" s="3"/>
-      <c r="B519" s="3"/>
-      <c r="C519" s="3"/>
+      <c r="A519" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44411.0)</f>
+        <v>44411</v>
+      </c>
+      <c r="B519" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.0)</f>
+        <v>26</v>
+      </c>
+      <c r="C519" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.857142857142854)</f>
+        <v>54.85714286</v>
+      </c>
     </row>
     <row r="520">
-      <c r="A520" s="3"/>
-      <c r="B520" s="3"/>
-      <c r="C520" s="3"/>
+      <c r="A520" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44412.0)</f>
+        <v>44412</v>
+      </c>
+      <c r="B520" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),59.0)</f>
+        <v>59</v>
+      </c>
+      <c r="C520" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.714285714285715)</f>
+        <v>52.71428571</v>
+      </c>
     </row>
     <row r="521">
-      <c r="A521" s="3"/>
-      <c r="B521" s="3"/>
-      <c r="C521" s="3"/>
+      <c r="A521" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44413.0)</f>
+        <v>44413</v>
+      </c>
+      <c r="B521" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),72.0)</f>
+        <v>72</v>
+      </c>
+      <c r="C521" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),53.714285714285715)</f>
+        <v>53.71428571</v>
+      </c>
     </row>
     <row r="522">
-      <c r="A522" s="3"/>
-      <c r="B522" s="3"/>
-      <c r="C522" s="3"/>
+      <c r="A522" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44414.0)</f>
+        <v>44414</v>
+      </c>
+      <c r="B522" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.0)</f>
+        <v>52</v>
+      </c>
+      <c r="C522" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.0)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="523">
-      <c r="A523" s="3"/>
+      <c r="A523" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44415.0)</f>
+        <v>44415</v>
+      </c>
       <c r="B523" s="3"/>
       <c r="C523" s="3"/>
     </row>
     <row r="524">
-      <c r="A524" s="3"/>
+      <c r="A524" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44416.0)</f>
+        <v>44416</v>
+      </c>
       <c r="B524" s="3"/>
       <c r="C524" s="3"/>
     </row>
     <row r="525">
-      <c r="A525" s="3"/>
-      <c r="B525" s="3"/>
-      <c r="C525" s="3"/>
+      <c r="A525" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44417.0)</f>
+        <v>44417</v>
+      </c>
+      <c r="B525" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),156.0)</f>
+        <v>156</v>
+      </c>
+      <c r="C525" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),52.142857142857146)</f>
+        <v>52.14285714</v>
+      </c>
     </row>
     <row r="526">
-      <c r="A526" s="3"/>
-      <c r="B526" s="3"/>
-      <c r="C526" s="3"/>
+      <c r="A526" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44418.0)</f>
+        <v>44418</v>
+      </c>
+      <c r="B526" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),35.0)</f>
+        <v>35</v>
+      </c>
+      <c r="C526" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),53.42857142857143)</f>
+        <v>53.42857143</v>
+      </c>
     </row>
     <row r="527">
-      <c r="A527" s="3"/>
-      <c r="B527" s="3"/>
-      <c r="C527" s="3"/>
+      <c r="A527" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44419.0)</f>
+        <v>44419</v>
+      </c>
+      <c r="B527" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),80.0)</f>
+        <v>80</v>
+      </c>
+      <c r="C527" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),56.42857142857143)</f>
+        <v>56.42857143</v>
+      </c>
     </row>
     <row r="528">
-      <c r="A528" s="3"/>
-      <c r="B528" s="3"/>
-      <c r="C528" s="3"/>
+      <c r="A528" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44420.0)</f>
+        <v>44420</v>
+      </c>
+      <c r="B528" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),86.0)</f>
+        <v>86</v>
+      </c>
+      <c r="C528" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),58.42857142857143)</f>
+        <v>58.42857143</v>
+      </c>
     </row>
     <row r="529">
-      <c r="A529" s="3"/>
-      <c r="B529" s="3"/>
-      <c r="C529" s="3"/>
+      <c r="A529" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44421.0)</f>
+        <v>44421</v>
+      </c>
+      <c r="B529" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),104.0)</f>
+        <v>104</v>
+      </c>
+      <c r="C529" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.85714285714286)</f>
+        <v>65.85714286</v>
+      </c>
     </row>
     <row r="530">
-      <c r="A530" s="3"/>
+      <c r="A530" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44422.0)</f>
+        <v>44422</v>
+      </c>
       <c r="B530" s="3"/>
       <c r="C530" s="3"/>
     </row>
     <row r="531">
-      <c r="A531" s="3"/>
+      <c r="A531" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44423.0)</f>
+        <v>44423</v>
+      </c>
       <c r="B531" s="3"/>
       <c r="C531" s="3"/>
     </row>
     <row r="532">
-      <c r="A532" s="3"/>
-      <c r="B532" s="3"/>
-      <c r="C532" s="3"/>
+      <c r="A532" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44424.0)</f>
+        <v>44424</v>
+      </c>
+      <c r="B532" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),188.0)</f>
+        <v>188</v>
+      </c>
+      <c r="C532" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),70.42857142857143)</f>
+        <v>70.42857143</v>
+      </c>
     </row>
     <row r="533">
-      <c r="A533" s="3"/>
-      <c r="B533" s="3"/>
-      <c r="C533" s="3"/>
+      <c r="A533" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44425.0)</f>
+        <v>44425</v>
+      </c>
+      <c r="B533" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45.0)</f>
+        <v>45</v>
+      </c>
+      <c r="C533" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.85714285714286)</f>
+        <v>71.85714286</v>
+      </c>
     </row>
     <row r="534">
-      <c r="A534" s="3"/>
-      <c r="B534" s="3"/>
-      <c r="C534" s="3"/>
+      <c r="A534" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44426.0)</f>
+        <v>44426</v>
+      </c>
+      <c r="B534" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),109.0)</f>
+        <v>109</v>
+      </c>
+      <c r="C534" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),76.0)</f>
+        <v>76</v>
+      </c>
     </row>
     <row r="535">
-      <c r="A535" s="3"/>
-      <c r="B535" s="3"/>
-      <c r="C535" s="3"/>
+      <c r="A535" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44427.0)</f>
+        <v>44427</v>
+      </c>
+      <c r="B535" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),123.0)</f>
+        <v>123</v>
+      </c>
+      <c r="C535" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),81.28571428571429)</f>
+        <v>81.28571429</v>
+      </c>
     </row>
     <row r="536">
-      <c r="A536" s="3"/>
+      <c r="A536" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44428.0)</f>
+        <v>44428</v>
+      </c>
       <c r="B536" s="3"/>
       <c r="C536" s="3"/>
     </row>
     <row r="537">
-      <c r="A537" s="3"/>
+      <c r="A537" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44429.0)</f>
+        <v>44429</v>
+      </c>
       <c r="B537" s="3"/>
       <c r="C537" s="3"/>
     </row>
     <row r="538">
-      <c r="A538" s="3"/>
+      <c r="A538" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44430.0)</f>
+        <v>44430</v>
+      </c>
       <c r="B538" s="3"/>
       <c r="C538" s="3"/>
     </row>
     <row r="539">
-      <c r="A539" s="3"/>
-      <c r="B539" s="3"/>
-      <c r="C539" s="3"/>
+      <c r="A539" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44431.0)</f>
+        <v>44431</v>
+      </c>
+      <c r="B539" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),340.0)</f>
+        <v>340</v>
+      </c>
+      <c r="C539" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),88.14285714285714)</f>
+        <v>88.14285714</v>
+      </c>
     </row>
     <row r="540">
-      <c r="A540" s="3"/>
-      <c r="B540" s="3"/>
-      <c r="C540" s="3"/>
+      <c r="A540" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44432.0)</f>
+        <v>44432</v>
+      </c>
+      <c r="B540" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),82.0)</f>
+        <v>82</v>
+      </c>
+      <c r="C540" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),93.42857142857143)</f>
+        <v>93.42857143</v>
+      </c>
     </row>
     <row r="541">
-      <c r="A541" s="3"/>
-      <c r="B541" s="3"/>
-      <c r="C541" s="3"/>
+      <c r="A541" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44433.0)</f>
+        <v>44433</v>
+      </c>
+      <c r="B541" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),134.0)</f>
+        <v>134</v>
+      </c>
+      <c r="C541" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),97.0)</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="542">
-      <c r="A542" s="3"/>
-      <c r="B542" s="3"/>
-      <c r="C542" s="3"/>
+      <c r="A542" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44434.0)</f>
+        <v>44434</v>
+      </c>
+      <c r="B542" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),180.0)</f>
+        <v>180</v>
+      </c>
+      <c r="C542" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),105.14285714285714)</f>
+        <v>105.1428571</v>
+      </c>
     </row>
     <row r="543">
-      <c r="A543" s="3"/>
-      <c r="B543" s="3"/>
-      <c r="C543" s="3"/>
+      <c r="A543" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44435.0)</f>
+        <v>44435</v>
+      </c>
+      <c r="B543" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),189.0)</f>
+        <v>189</v>
+      </c>
+      <c r="C543" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),132.14285714285714)</f>
+        <v>132.1428571</v>
+      </c>
     </row>
     <row r="544">
-      <c r="A544" s="3"/>
+      <c r="A544" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44436.0)</f>
+        <v>44436</v>
+      </c>
       <c r="B544" s="3"/>
       <c r="C544" s="3"/>
     </row>
     <row r="545">
-      <c r="A545" s="3"/>
+      <c r="A545" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44437.0)</f>
+        <v>44437</v>
+      </c>
       <c r="B545" s="3"/>
       <c r="C545" s="3"/>
     </row>
     <row r="546">
-      <c r="A546" s="3"/>
-      <c r="B546" s="3"/>
-      <c r="C546" s="3"/>
+      <c r="A546" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44438.0)</f>
+        <v>44438</v>
+      </c>
+      <c r="B546" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),521.0)</f>
+        <v>521</v>
+      </c>
+      <c r="C546" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),158.0)</f>
+        <v>158</v>
+      </c>
     </row>
     <row r="547">
-      <c r="A547" s="3"/>
-      <c r="B547" s="3"/>
-      <c r="C547" s="3"/>
+      <c r="A547" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44439.0)</f>
+        <v>44439</v>
+      </c>
+      <c r="B547" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),110.0)</f>
+        <v>110</v>
+      </c>
+      <c r="C547" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),162.0)</f>
+        <v>162</v>
+      </c>
     </row>
     <row r="548">
-      <c r="A548" s="3"/>
-      <c r="B548" s="3"/>
-      <c r="C548" s="3"/>
+      <c r="A548" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44440.0)</f>
+        <v>44440</v>
+      </c>
+      <c r="B548" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),194.0)</f>
+        <v>194</v>
+      </c>
+      <c r="C548" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),170.57142857142858)</f>
+        <v>170.5714286</v>
+      </c>
     </row>
     <row r="549">
-      <c r="A549" s="3"/>
-      <c r="B549" s="3"/>
-      <c r="C549" s="3"/>
+      <c r="A549" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44441.0)</f>
+        <v>44441</v>
+      </c>
+      <c r="B549" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),262.0)</f>
+        <v>262</v>
+      </c>
+      <c r="C549" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),182.28571428571428)</f>
+        <v>182.2857143</v>
+      </c>
     </row>
     <row r="550">
-      <c r="A550" s="3"/>
-      <c r="B550" s="3"/>
-      <c r="C550" s="3"/>
+      <c r="A550" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44442.0)</f>
+        <v>44442</v>
+      </c>
+      <c r="B550" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),247.0)</f>
+        <v>247</v>
+      </c>
+      <c r="C550" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),190.57142857142858)</f>
+        <v>190.5714286</v>
+      </c>
     </row>
     <row r="551">
-      <c r="A551" s="3"/>
+      <c r="A551" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44443.0)</f>
+        <v>44443</v>
+      </c>
       <c r="B551" s="3"/>
       <c r="C551" s="3"/>
     </row>
     <row r="552">
-      <c r="A552" s="3"/>
+      <c r="A552" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44444.0)</f>
+        <v>44444</v>
+      </c>
       <c r="B552" s="3"/>
       <c r="C552" s="3"/>
     </row>
     <row r="553">
-      <c r="A553" s="3"/>
-      <c r="B553" s="3"/>
-      <c r="C553" s="3"/>
+      <c r="A553" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44445.0)</f>
+        <v>44445</v>
+      </c>
+      <c r="B553" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),648.0)</f>
+        <v>648</v>
+      </c>
+      <c r="C553" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),208.71428571428572)</f>
+        <v>208.7142857</v>
+      </c>
     </row>
     <row r="554">
-      <c r="A554" s="3"/>
-      <c r="B554" s="3"/>
-      <c r="C554" s="3"/>
+      <c r="A554" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44446.0)</f>
+        <v>44446</v>
+      </c>
+      <c r="B554" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),130.0)</f>
+        <v>130</v>
+      </c>
+      <c r="C554" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),211.57142857142858)</f>
+        <v>211.5714286</v>
+      </c>
     </row>
     <row r="555">
-      <c r="A555" s="3"/>
-      <c r="B555" s="3"/>
-      <c r="C555" s="3"/>
+      <c r="A555" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44447.0)</f>
+        <v>44447</v>
+      </c>
+      <c r="B555" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),246.0)</f>
+        <v>246</v>
+      </c>
+      <c r="C555" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),219.0)</f>
+        <v>219</v>
+      </c>
     </row>
     <row r="556">
-      <c r="A556" s="3"/>
-      <c r="B556" s="3"/>
-      <c r="C556" s="3"/>
+      <c r="A556" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44448.0)</f>
+        <v>44448</v>
+      </c>
+      <c r="B556" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),345.0)</f>
+        <v>345</v>
+      </c>
+      <c r="C556" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),230.85714285714286)</f>
+        <v>230.8571429</v>
+      </c>
     </row>
     <row r="557">
-      <c r="A557" s="3"/>
-      <c r="B557" s="3"/>
-      <c r="C557" s="3"/>
+      <c r="A557" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44449.0)</f>
+        <v>44449</v>
+      </c>
+      <c r="B557" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),323.0)</f>
+        <v>323</v>
+      </c>
+      <c r="C557" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),241.71428571428572)</f>
+        <v>241.7142857</v>
+      </c>
     </row>
     <row r="558">
-      <c r="A558" s="3"/>
+      <c r="A558" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44450.0)</f>
+        <v>44450</v>
+      </c>
       <c r="B558" s="3"/>
       <c r="C558" s="3"/>
     </row>
     <row r="559">
-      <c r="A559" s="3"/>
+      <c r="A559" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44451.0)</f>
+        <v>44451</v>
+      </c>
       <c r="B559" s="3"/>
       <c r="C559" s="3"/>
     </row>
     <row r="560">
-      <c r="A560" s="3"/>
-      <c r="B560" s="3"/>
-      <c r="C560" s="3"/>
+      <c r="A560" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44452.0)</f>
+        <v>44452</v>
+      </c>
+      <c r="B560" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),873.0)</f>
+        <v>873</v>
+      </c>
+      <c r="C560" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),273.85714285714283)</f>
+        <v>273.8571429</v>
+      </c>
     </row>
     <row r="561">
-      <c r="A561" s="3"/>
-      <c r="B561" s="3"/>
-      <c r="C561" s="3"/>
+      <c r="A561" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44453.0)</f>
+        <v>44453</v>
+      </c>
+      <c r="B561" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),246.0)</f>
+        <v>246</v>
+      </c>
+      <c r="C561" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),290.42857142857144)</f>
+        <v>290.4285714</v>
+      </c>
     </row>
     <row r="562">
-      <c r="A562" s="3"/>
-      <c r="B562" s="3"/>
-      <c r="C562" s="3"/>
+      <c r="A562" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44454.0)</f>
+        <v>44454</v>
+      </c>
+      <c r="B562" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),371.0)</f>
+        <v>371</v>
+      </c>
+      <c r="C562" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),308.2857142857143)</f>
+        <v>308.2857143</v>
+      </c>
     </row>
     <row r="563">
-      <c r="A563" s="3"/>
-      <c r="B563" s="3"/>
-      <c r="C563" s="3"/>
+      <c r="A563" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44455.0)</f>
+        <v>44455</v>
+      </c>
+      <c r="B563" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),458.0)</f>
+        <v>458</v>
+      </c>
+      <c r="C563" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),324.42857142857144)</f>
+        <v>324.4285714</v>
+      </c>
     </row>
     <row r="564">
-      <c r="A564" s="3"/>
-      <c r="B564" s="3"/>
-      <c r="C564" s="3"/>
+      <c r="A564" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44456.0)</f>
+        <v>44456</v>
+      </c>
+      <c r="B564" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),479.0)</f>
+        <v>479</v>
+      </c>
+      <c r="C564" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),346.7142857142857)</f>
+        <v>346.7142857</v>
+      </c>
     </row>
     <row r="565">
-      <c r="A565" s="3"/>
+      <c r="A565" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44457.0)</f>
+        <v>44457</v>
+      </c>
       <c r="B565" s="3"/>
       <c r="C565" s="3"/>
     </row>
     <row r="566">
-      <c r="A566" s="3"/>
+      <c r="A566" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44458.0)</f>
+        <v>44458</v>
+      </c>
       <c r="B566" s="3"/>
       <c r="C566" s="3"/>
     </row>
     <row r="567">
-      <c r="A567" s="3"/>
-      <c r="B567" s="3"/>
-      <c r="C567" s="3"/>
+      <c r="A567" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44459.0)</f>
+        <v>44459</v>
+      </c>
+      <c r="B567" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1072.0)</f>
+        <v>1072</v>
+      </c>
+      <c r="C567" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),375.14285714285717)</f>
+        <v>375.1428571</v>
+      </c>
     </row>
     <row r="568">
-      <c r="A568" s="3"/>
-      <c r="B568" s="3"/>
-      <c r="C568" s="3"/>
+      <c r="A568" s="2">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44460.0)</f>
+        <v>44460</v>
+      </c>
+      <c r="B568" s="3">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),289.0)</f>
+        <v>289</v>
+      </c>
+      <c r="C568" s="4">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),381.2857142857143)</f>
+        <v>381.2857143</v>
+      </c>
     </row>
     <row r="569">
       <c r="A569" s="3"/>

</xml_diff>